<commit_message>
Small tweaking needed, and Notes
</commit_message>
<xml_diff>
--- a/Presentations/December 9, 2013/gaant.xlsx
+++ b/Presentations/December 9, 2013/gaant.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="17">
   <si>
     <t>Frame</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Assemble</t>
   </si>
   <si>
-    <t>Fixture</t>
-  </si>
-  <si>
     <t>Design</t>
   </si>
   <si>
@@ -58,13 +55,25 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Spec parts</t>
+  </si>
+  <si>
+    <t>Attach to frame</t>
+  </si>
+  <si>
+    <t>Calibrate</t>
+  </si>
+  <si>
+    <t>Attach to Frame</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +83,14 @@
     </font>
     <font>
       <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -115,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -127,15 +144,31 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -156,7 +189,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6"/>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -457,15 +490,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:AD22"/>
+  <dimension ref="D2:AD24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="21" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -474,7 +507,7 @@
     </row>
     <row r="5" spans="4:30" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="4">
         <v>41652</v>
@@ -554,7 +587,7 @@
       <c r="AD5" s="1"/>
     </row>
     <row r="6" spans="4:30" x14ac:dyDescent="0.25">
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="2"/>
@@ -576,14 +609,14 @@
       <c r="U6" s="2"/>
     </row>
     <row r="7" spans="4:30" x14ac:dyDescent="0.25">
-      <c r="D7" s="2" t="s">
-        <v>2</v>
+      <c r="D7" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -603,34 +636,26 @@
     </row>
     <row r="8" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="G8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
@@ -641,51 +666,57 @@
     </row>
     <row r="9" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="T9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
     </row>
     <row r="10" spans="4:30" x14ac:dyDescent="0.25">
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
+      <c r="K10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
@@ -697,7 +728,7 @@
     </row>
     <row r="11" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D11" s="2" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -708,25 +739,25 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
+      <c r="N11" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
+      <c r="S11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="U11" s="2"/>
     </row>
     <row r="12" spans="4:30" x14ac:dyDescent="0.25">
-      <c r="D12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -744,17 +775,13 @@
       <c r="U12" s="2"/>
     </row>
     <row r="13" spans="4:30" x14ac:dyDescent="0.25">
-      <c r="D13" s="2" t="s">
-        <v>6</v>
+      <c r="D13" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -771,30 +798,22 @@
     </row>
     <row r="14" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
@@ -805,49 +824,51 @@
     </row>
     <row r="15" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D15" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
-      <c r="O15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="T15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="U15" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
     </row>
     <row r="16" spans="4:30" x14ac:dyDescent="0.25">
-      <c r="D16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
+      <c r="H16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -861,17 +882,25 @@
     </row>
     <row r="17" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D17" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
+      <c r="J17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
@@ -882,12 +911,8 @@
       <c r="U17" s="2"/>
     </row>
     <row r="18" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -906,13 +931,11 @@
       <c r="U18" s="2"/>
     </row>
     <row r="19" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D19" s="2" t="s">
-        <v>10</v>
+      <c r="D19" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -931,22 +954,16 @@
     </row>
     <row r="20" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="F20" s="2"/>
-      <c r="G20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -964,23 +981,17 @@
         <v>9</v>
       </c>
       <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
@@ -991,51 +1002,113 @@
     </row>
     <row r="22" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D22" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
-      <c r="O22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="T22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="U22" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+    </row>
+    <row r="23" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+    </row>
+    <row r="24" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E6:U22">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
+  <conditionalFormatting sqref="E6:U24">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>